<commit_message>
scripts for preliminary figures 3, 4, and 5
</commit_message>
<xml_diff>
--- a/results/Oil preliminary/PCA/exploratory PCA results.xlsx
+++ b/results/Oil preliminary/PCA/exploratory PCA results.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Traits/Seed traits/Oil content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/results/Oil preliminary/PCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{52EB940A-A855-4E62-9993-921735BE7F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E4F43E7-3AF3-40E8-A924-258FAE00D688}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="8_{52EB940A-A855-4E62-9993-921735BE7F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F53B8E6A-26DA-48CD-A7AC-BCA68EBB1EA2}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{12EB29D1-3BF5-4131-9DFF-385521089C46}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{12EB29D1-3BF5-4131-9DFF-385521089C46}"/>
   </bookViews>
   <sheets>
     <sheet name="All variables" sheetId="1" r:id="rId1"/>
     <sheet name="out_correlated" sheetId="3" r:id="rId2"/>
     <sheet name="sin Teesdalia" sheetId="2" r:id="rId3"/>
     <sheet name="sin PERoil" sheetId="4" r:id="rId4"/>
+    <sheet name="FAME&gt;3%" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="82">
   <si>
     <t>Dim.1</t>
   </si>
@@ -346,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -363,8 +364,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,8 +734,149 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC68A659-140C-46C2-A2AA-58462620464F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1419225" y="8763000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8C0A1FB-2F83-48EC-BDA3-357FE229CEF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="9144000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>103948</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE1936BC-3664-DBE7-C12D-EC2A7F19A56A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8467726" y="85726"/>
+          <a:ext cx="6286500" cy="4209222"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{495B757E-E12C-4239-B62B-80C4F98D0D13}">
-  <dimension ref="A1:V47"/>
+  <dimension ref="A1:V95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD95"/>
+    <sheetView topLeftCell="D28" workbookViewId="0">
+      <selection sqref="A1:W49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3248,6 +3396,53 @@
         <v>1</v>
       </c>
     </row>
+    <row r="49" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="J1:J2"/>
@@ -4968,7 +5163,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L3" s="8"/>
+      <c r="L3" s="1"/>
       <c r="M3" t="s">
         <v>0</v>
       </c>
@@ -4984,7 +5179,7 @@
       <c r="Q3" t="s">
         <v>4</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="1" t="s">
         <v>81</v>
       </c>
       <c r="T3" t="s">
@@ -4998,7 +5193,7 @@
       </c>
     </row>
     <row r="4" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="1" t="s">
         <v>73</v>
       </c>
       <c r="M4" s="2">
@@ -5016,7 +5211,7 @@
       <c r="Q4" s="2">
         <v>0.94709520999999997</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="S4" s="1" t="s">
         <v>55</v>
       </c>
       <c r="T4" s="2">
@@ -5030,7 +5225,7 @@
       </c>
     </row>
     <row r="5" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="M5" s="2">
@@ -5048,7 +5243,7 @@
       <c r="Q5" s="2">
         <v>0.12433093000000001</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="S5" s="1" t="s">
         <v>56</v>
       </c>
       <c r="T5" s="2">
@@ -5062,7 +5257,7 @@
       </c>
     </row>
     <row r="6" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M6" s="2">
@@ -5080,7 +5275,7 @@
       <c r="Q6" s="2">
         <v>2.49996961</v>
       </c>
-      <c r="S6" s="8" t="s">
+      <c r="S6" s="1" t="s">
         <v>57</v>
       </c>
       <c r="T6" s="2">
@@ -5094,7 +5289,7 @@
       </c>
     </row>
     <row r="7" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="2">
@@ -5112,7 +5307,7 @@
       <c r="Q7" s="2">
         <v>5.21029097</v>
       </c>
-      <c r="S7" s="8" t="s">
+      <c r="S7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="T7" s="2">
@@ -5126,7 +5321,7 @@
       </c>
     </row>
     <row r="8" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L8" s="8" t="s">
+      <c r="L8" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M8" s="2">
@@ -5144,7 +5339,7 @@
       <c r="Q8" s="2">
         <v>9.9708478199999995</v>
       </c>
-      <c r="S8" s="8" t="s">
+      <c r="S8" s="1" t="s">
         <v>59</v>
       </c>
       <c r="T8" s="2">
@@ -5158,7 +5353,7 @@
       </c>
     </row>
     <row r="9" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M9" s="2">
@@ -5176,7 +5371,7 @@
       <c r="Q9" s="2">
         <v>6.7039595299999997</v>
       </c>
-      <c r="S9" s="8" t="s">
+      <c r="S9" s="1" t="s">
         <v>60</v>
       </c>
       <c r="T9" s="2">
@@ -5190,7 +5385,7 @@
       </c>
     </row>
     <row r="10" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M10" s="2">
@@ -5208,7 +5403,7 @@
       <c r="Q10" s="2">
         <v>16.527833780000002</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="1" t="s">
         <v>61</v>
       </c>
       <c r="T10" s="2">
@@ -5222,7 +5417,7 @@
       </c>
     </row>
     <row r="11" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="1" t="s">
         <v>42</v>
       </c>
       <c r="M11" s="2">
@@ -5240,7 +5435,7 @@
       <c r="Q11" s="2">
         <v>14.117322619999999</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="S11" s="1" t="s">
         <v>62</v>
       </c>
       <c r="T11" s="2">
@@ -5254,7 +5449,7 @@
       </c>
     </row>
     <row r="12" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M12" s="2">
@@ -5272,7 +5467,7 @@
       <c r="Q12" s="2">
         <v>10.63667579</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="S12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="T12" s="2">
@@ -5286,7 +5481,7 @@
       </c>
     </row>
     <row r="13" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L13" s="8" t="s">
+      <c r="L13" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M13" s="2">
@@ -5304,7 +5499,7 @@
       <c r="Q13" s="2">
         <v>7.9209974599999997</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="S13" s="1" t="s">
         <v>64</v>
       </c>
       <c r="T13" s="2">
@@ -5318,7 +5513,7 @@
       </c>
     </row>
     <row r="14" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M14" s="2">
@@ -5336,7 +5531,7 @@
       <c r="Q14" s="2">
         <v>1.621423E-2</v>
       </c>
-      <c r="S14" s="8" t="s">
+      <c r="S14" s="1" t="s">
         <v>65</v>
       </c>
       <c r="T14" s="2">
@@ -5350,7 +5545,7 @@
       </c>
     </row>
     <row r="15" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M15" s="2">
@@ -5368,7 +5563,7 @@
       <c r="Q15" s="2">
         <v>7.4177125999999998</v>
       </c>
-      <c r="S15" s="8" t="s">
+      <c r="S15" s="1" t="s">
         <v>66</v>
       </c>
       <c r="T15" s="2">
@@ -5382,7 +5577,7 @@
       </c>
     </row>
     <row r="16" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="1" t="s">
         <v>47</v>
       </c>
       <c r="M16" s="2">
@@ -5400,7 +5595,7 @@
       <c r="Q16" s="2">
         <v>7.2558070000000002E-2</v>
       </c>
-      <c r="S16" s="8" t="s">
+      <c r="S16" s="1" t="s">
         <v>67</v>
       </c>
       <c r="T16" s="2">
@@ -5414,7 +5609,7 @@
       </c>
     </row>
     <row r="17" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="1" t="s">
         <v>48</v>
       </c>
       <c r="M17" s="2">
@@ -5432,7 +5627,7 @@
       <c r="Q17" s="2">
         <v>4.52470953</v>
       </c>
-      <c r="S17" s="8" t="s">
+      <c r="S17" s="1" t="s">
         <v>68</v>
       </c>
       <c r="T17" s="2">
@@ -5446,7 +5641,7 @@
       </c>
     </row>
     <row r="18" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L18" s="8" t="s">
+      <c r="L18" s="1" t="s">
         <v>74</v>
       </c>
       <c r="M18" s="2">
@@ -5464,7 +5659,7 @@
       <c r="Q18" s="2">
         <v>1.91841577</v>
       </c>
-      <c r="S18" s="8" t="s">
+      <c r="S18" s="1" t="s">
         <v>69</v>
       </c>
       <c r="T18" s="2">
@@ -5478,7 +5673,7 @@
       </c>
     </row>
     <row r="19" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L19" s="8" t="s">
+      <c r="L19" s="1" t="s">
         <v>75</v>
       </c>
       <c r="M19" s="2">
@@ -5496,7 +5691,7 @@
       <c r="Q19" s="2">
         <v>7.4326870000000003E-2</v>
       </c>
-      <c r="S19" s="8" t="s">
+      <c r="S19" s="1" t="s">
         <v>70</v>
       </c>
       <c r="T19" s="2">
@@ -5510,7 +5705,7 @@
       </c>
     </row>
     <row r="20" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L20" s="8" t="s">
+      <c r="L20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M20" s="2">
@@ -5528,7 +5723,7 @@
       <c r="Q20" s="2">
         <v>5.1242601800000003</v>
       </c>
-      <c r="S20" s="8" t="s">
+      <c r="S20" s="1" t="s">
         <v>71</v>
       </c>
       <c r="T20" s="2">
@@ -5542,7 +5737,7 @@
       </c>
     </row>
     <row r="21" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L21" s="8" t="s">
+      <c r="L21" s="1" t="s">
         <v>50</v>
       </c>
       <c r="M21" s="2">
@@ -5560,7 +5755,7 @@
       <c r="Q21" s="2">
         <v>5.9507455699999996</v>
       </c>
-      <c r="S21" s="8" t="s">
+      <c r="S21" s="1" t="s">
         <v>77</v>
       </c>
       <c r="T21" s="2">
@@ -5574,7 +5769,7 @@
       </c>
     </row>
     <row r="22" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L22" s="8" t="s">
+      <c r="L22" s="1" t="s">
         <v>76</v>
       </c>
       <c r="M22" s="2">
@@ -5592,7 +5787,7 @@
       <c r="Q22" s="2">
         <v>0</v>
       </c>
-      <c r="S22" s="8" t="s">
+      <c r="S22" s="1" t="s">
         <v>78</v>
       </c>
       <c r="T22" s="2">
@@ -5606,7 +5801,7 @@
       </c>
     </row>
     <row r="23" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L23" s="8" t="s">
+      <c r="L23" s="1" t="s">
         <v>51</v>
       </c>
       <c r="M23" s="2">
@@ -5624,7 +5819,7 @@
       <c r="Q23" s="2">
         <v>1.897426E-2</v>
       </c>
-      <c r="S23" s="8" t="s">
+      <c r="S23" s="1" t="s">
         <v>79</v>
       </c>
       <c r="T23" s="2">
@@ -5638,7 +5833,7 @@
       </c>
     </row>
     <row r="24" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L24" s="8" t="s">
+      <c r="L24" s="1" t="s">
         <v>52</v>
       </c>
       <c r="M24" s="2">
@@ -5656,7 +5851,7 @@
       <c r="Q24" s="2">
         <v>0.22275918</v>
       </c>
-      <c r="S24" s="8" t="s">
+      <c r="S24" s="1" t="s">
         <v>80</v>
       </c>
       <c r="T24" s="2">
@@ -5670,7 +5865,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="1"/>
       <c r="B35" t="s">
         <v>73</v>
       </c>
@@ -5733,7 +5928,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B36">
@@ -5798,7 +5993,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B37">
@@ -5863,7 +6058,7 @@
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B38">
@@ -5928,7 +6123,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B39">
@@ -5993,7 +6188,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B40">
@@ -6058,7 +6253,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B41">
@@ -6123,7 +6318,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B42">
@@ -6188,7 +6383,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B43">
@@ -6253,7 +6448,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B44">
@@ -6318,7 +6513,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B45">
@@ -6383,7 +6578,7 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B46">
@@ -6448,7 +6643,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B47">
@@ -6513,7 +6708,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B48">
@@ -6578,7 +6773,7 @@
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B49">
@@ -6643,7 +6838,7 @@
       </c>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B50">
@@ -6708,7 +6903,7 @@
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B51">
@@ -6773,7 +6968,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B52">
@@ -6838,7 +7033,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B53">
@@ -6903,7 +7098,7 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
+      <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B54">
@@ -6968,7 +7163,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
+      <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B55">
@@ -7033,16 +7228,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M4:Q24">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B36:U55">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -7052,6 +7237,16 @@
         <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:Q24">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -7071,7 +7266,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L2" s="8"/>
+      <c r="L2" s="1"/>
       <c r="M2" t="s">
         <v>0</v>
       </c>
@@ -7087,7 +7282,7 @@
       <c r="Q2" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="8"/>
+      <c r="S2" s="1"/>
       <c r="T2" t="s">
         <v>53</v>
       </c>
@@ -7099,7 +7294,7 @@
       </c>
     </row>
     <row r="3" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="1" t="s">
         <v>73</v>
       </c>
       <c r="M3" s="2">
@@ -7117,7 +7312,7 @@
       <c r="Q3" s="2">
         <v>0.89616150000000006</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="1" t="s">
         <v>55</v>
       </c>
       <c r="T3" s="2">
@@ -7131,7 +7326,7 @@
       </c>
     </row>
     <row r="4" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="M4" s="2">
@@ -7149,7 +7344,7 @@
       <c r="Q4" s="2">
         <v>5.585677E-2</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="S4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="T4" s="2">
@@ -7163,7 +7358,7 @@
       </c>
     </row>
     <row r="5" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="M5" s="2">
@@ -7181,7 +7376,7 @@
       <c r="Q5" s="2">
         <v>2.0948500000000001</v>
       </c>
-      <c r="S5" s="8" t="s">
+      <c r="S5" s="1" t="s">
         <v>57</v>
       </c>
       <c r="T5" s="2">
@@ -7195,7 +7390,7 @@
       </c>
     </row>
     <row r="6" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="2">
@@ -7213,7 +7408,7 @@
       <c r="Q6" s="2">
         <v>4.5129539999999997</v>
       </c>
-      <c r="S6" s="8" t="s">
+      <c r="S6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="T6" s="2">
@@ -7227,7 +7422,7 @@
       </c>
     </row>
     <row r="7" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M7" s="2">
@@ -7245,7 +7440,7 @@
       <c r="Q7" s="2">
         <v>9.7415430000000001</v>
       </c>
-      <c r="S7" s="8" t="s">
+      <c r="S7" s="1" t="s">
         <v>59</v>
       </c>
       <c r="T7" s="2">
@@ -7259,7 +7454,7 @@
       </c>
     </row>
     <row r="8" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L8" s="8" t="s">
+      <c r="L8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="M8" s="2">
@@ -7277,7 +7472,7 @@
       <c r="Q8" s="2">
         <v>6.2980520000000002</v>
       </c>
-      <c r="S8" s="8" t="s">
+      <c r="S8" s="1" t="s">
         <v>60</v>
       </c>
       <c r="T8" s="2">
@@ -7291,7 +7486,7 @@
       </c>
     </row>
     <row r="9" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M9" s="2">
@@ -7309,7 +7504,7 @@
       <c r="Q9" s="2">
         <v>19.21941</v>
       </c>
-      <c r="S9" s="8" t="s">
+      <c r="S9" s="1" t="s">
         <v>61</v>
       </c>
       <c r="T9" s="2">
@@ -7323,7 +7518,7 @@
       </c>
     </row>
     <row r="10" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L10" s="8" t="s">
+      <c r="L10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="M10" s="2">
@@ -7341,7 +7536,7 @@
       <c r="Q10" s="2">
         <v>13.72203</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="1" t="s">
         <v>62</v>
       </c>
       <c r="T10" s="2">
@@ -7355,7 +7550,7 @@
       </c>
     </row>
     <row r="11" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L11" s="8" t="s">
+      <c r="L11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M11" s="2">
@@ -7373,7 +7568,7 @@
       <c r="Q11" s="2">
         <v>10.88932</v>
       </c>
-      <c r="S11" s="8" t="s">
+      <c r="S11" s="1" t="s">
         <v>63</v>
       </c>
       <c r="T11" s="2">
@@ -7387,7 +7582,7 @@
       </c>
     </row>
     <row r="12" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="1" t="s">
         <v>44</v>
       </c>
       <c r="M12" s="2">
@@ -7405,7 +7600,7 @@
       <c r="Q12" s="2">
         <v>9.0445100000000007</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="S12" s="1" t="s">
         <v>64</v>
       </c>
       <c r="T12" s="2">
@@ -7419,7 +7614,7 @@
       </c>
     </row>
     <row r="13" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L13" s="8" t="s">
+      <c r="L13" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M13" s="2">
@@ -7437,7 +7632,7 @@
       <c r="Q13" s="2">
         <v>5.7747710000000001E-2</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="S13" s="1" t="s">
         <v>65</v>
       </c>
       <c r="T13" s="2">
@@ -7451,7 +7646,7 @@
       </c>
     </row>
     <row r="14" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L14" s="8" t="s">
+      <c r="L14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="M14" s="2">
@@ -7469,7 +7664,7 @@
       <c r="Q14" s="2">
         <v>6.788043</v>
       </c>
-      <c r="S14" s="8" t="s">
+      <c r="S14" s="1" t="s">
         <v>66</v>
       </c>
       <c r="T14" s="2">
@@ -7483,7 +7678,7 @@
       </c>
     </row>
     <row r="15" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="1" t="s">
         <v>47</v>
       </c>
       <c r="M15" s="2">
@@ -7501,7 +7696,7 @@
       <c r="Q15" s="2">
         <v>1.9052930000000001E-4</v>
       </c>
-      <c r="S15" s="8" t="s">
+      <c r="S15" s="1" t="s">
         <v>67</v>
       </c>
       <c r="T15" s="2">
@@ -7515,7 +7710,7 @@
       </c>
     </row>
     <row r="16" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="1" t="s">
         <v>48</v>
       </c>
       <c r="M16" s="2">
@@ -7533,7 +7728,7 @@
       <c r="Q16" s="2">
         <v>4.123729</v>
       </c>
-      <c r="S16" s="8" t="s">
+      <c r="S16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="T16" s="2">
@@ -7547,7 +7742,7 @@
       </c>
     </row>
     <row r="17" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="1" t="s">
         <v>74</v>
       </c>
       <c r="M17" s="2">
@@ -7565,7 +7760,7 @@
       <c r="Q17" s="2">
         <v>1.8635219999999999</v>
       </c>
-      <c r="S17" s="8" t="s">
+      <c r="S17" s="1" t="s">
         <v>69</v>
       </c>
       <c r="T17" s="2">
@@ -7579,7 +7774,7 @@
       </c>
     </row>
     <row r="18" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L18" s="8" t="s">
+      <c r="L18" s="1" t="s">
         <v>75</v>
       </c>
       <c r="M18" s="2">
@@ -7597,7 +7792,7 @@
       <c r="Q18" s="2">
         <v>3.9156209999999997E-2</v>
       </c>
-      <c r="S18" s="8" t="s">
+      <c r="S18" s="1" t="s">
         <v>70</v>
       </c>
       <c r="T18" s="2">
@@ -7611,7 +7806,7 @@
       </c>
     </row>
     <row r="19" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L19" s="8" t="s">
+      <c r="L19" s="1" t="s">
         <v>49</v>
       </c>
       <c r="M19" s="2">
@@ -7629,7 +7824,7 @@
       <c r="Q19" s="2">
         <v>3.5575920000000001</v>
       </c>
-      <c r="S19" s="8" t="s">
+      <c r="S19" s="1" t="s">
         <v>71</v>
       </c>
       <c r="T19" s="2">
@@ -7643,7 +7838,7 @@
       </c>
     </row>
     <row r="20" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L20" s="8" t="s">
+      <c r="L20" s="1" t="s">
         <v>50</v>
       </c>
       <c r="M20" s="2">
@@ -7661,7 +7856,7 @@
       <c r="Q20" s="2">
         <v>6.7762890000000002</v>
       </c>
-      <c r="S20" s="8" t="s">
+      <c r="S20" s="1" t="s">
         <v>77</v>
       </c>
       <c r="T20" s="2">
@@ -7675,7 +7870,7 @@
       </c>
     </row>
     <row r="21" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L21" s="8" t="s">
+      <c r="L21" s="1" t="s">
         <v>76</v>
       </c>
       <c r="M21" s="2">
@@ -7693,7 +7888,7 @@
       <c r="Q21" s="2">
         <v>0</v>
       </c>
-      <c r="S21" s="8" t="s">
+      <c r="S21" s="1" t="s">
         <v>78</v>
       </c>
       <c r="T21" s="2">
@@ -7707,7 +7902,7 @@
       </c>
     </row>
     <row r="22" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L22" s="8" t="s">
+      <c r="L22" s="1" t="s">
         <v>51</v>
       </c>
       <c r="M22" s="2">
@@ -7725,7 +7920,7 @@
       <c r="Q22" s="2">
         <v>0.31904169999999998</v>
       </c>
-      <c r="S22" s="8" t="s">
+      <c r="S22" s="1" t="s">
         <v>79</v>
       </c>
       <c r="T22" s="2">
@@ -7739,7 +7934,7 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="1"/>
       <c r="B34" t="s">
         <v>73</v>
       </c>
@@ -7799,7 +7994,7 @@
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B35">
@@ -7861,7 +8056,7 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B36">
@@ -7923,7 +8118,7 @@
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B37">
@@ -7985,7 +8180,7 @@
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B38">
@@ -8047,7 +8242,7 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B39">
@@ -8109,7 +8304,7 @@
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B40">
@@ -8171,7 +8366,7 @@
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B41">
@@ -8233,7 +8428,7 @@
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B42">
@@ -8295,7 +8490,7 @@
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B43">
@@ -8357,7 +8552,7 @@
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B44">
@@ -8419,7 +8614,7 @@
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B45">
@@ -8481,7 +8676,7 @@
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B46">
@@ -8543,7 +8738,7 @@
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
+      <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B47">
@@ -8605,7 +8800,7 @@
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+      <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B48">
@@ -8667,7 +8862,7 @@
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B49">
@@ -8729,7 +8924,7 @@
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B50">
@@ -8791,7 +8986,7 @@
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B51">
@@ -8853,7 +9048,7 @@
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
+      <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B52">
@@ -8915,7 +9110,7 @@
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B53">
@@ -8977,6 +9172,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B35:T53">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M3:Q22">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -8987,8 +9194,705 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:T53">
-    <cfRule type="colorScale" priority="1">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83371D3-0EB2-44DF-8B67-7090F049F91E}">
+  <dimension ref="A1:W25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2">
+        <v>11.0085368</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.30324446999999999</v>
+      </c>
+      <c r="D3" s="2">
+        <v>32.4305679</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.4275074500000002</v>
+      </c>
+      <c r="F3" s="2">
+        <v>12.780138355</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2.3984397917</v>
+      </c>
+      <c r="J3" s="2">
+        <v>26.649331019000002</v>
+      </c>
+      <c r="K3" s="2">
+        <v>26.649329999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.3420118000000001</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.3036278499999998</v>
+      </c>
+      <c r="D4" s="2">
+        <v>32.529500499999997</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.7611847999999997</v>
+      </c>
+      <c r="F4" s="2">
+        <v>16.708949452999999</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2.1539176963000002</v>
+      </c>
+      <c r="J4" s="2">
+        <v>23.932418847000001</v>
+      </c>
+      <c r="K4" s="2">
+        <v>50.58175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5.7781919000000004</v>
+      </c>
+      <c r="C5" s="2">
+        <v>11.27421599</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7.6562840999999997</v>
+      </c>
+      <c r="E5" s="2">
+        <v>35.459855050000002</v>
+      </c>
+      <c r="F5" s="2">
+        <v>9.2068527489999994</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.2650747846999999</v>
+      </c>
+      <c r="J5" s="2">
+        <v>14.056386497</v>
+      </c>
+      <c r="K5" s="2">
+        <v>64.638140000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="2">
+        <v>14.859105</v>
+      </c>
+      <c r="C6" s="2">
+        <v>7.8350234600000004</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.2332505999999999</v>
+      </c>
+      <c r="E6" s="2">
+        <v>19.421773340000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>10.968075292</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1.1005766108999999</v>
+      </c>
+      <c r="J6" s="2">
+        <v>12.228629010000001</v>
+      </c>
+      <c r="K6" s="2">
+        <v>76.866770000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="2">
+        <v>31.006616099999999</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4.1562115200000003</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7.5996452999999997</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.98554176000000004</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.357374557</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.98313830489999998</v>
+      </c>
+      <c r="J7" s="2">
+        <v>10.923758942999999</v>
+      </c>
+      <c r="K7" s="2">
+        <v>87.790520000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7.1130692</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4.0161759999999998E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.71255900000000005</v>
+      </c>
+      <c r="E8" s="2">
+        <v>12.28729586</v>
+      </c>
+      <c r="F8" s="2">
+        <v>41.808568018999999</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.74240260790000001</v>
+      </c>
+      <c r="J8" s="2">
+        <v>8.2489178659999993</v>
+      </c>
+      <c r="K8" s="2">
+        <v>96.039439999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.99068979999999995</v>
+      </c>
+      <c r="C9" s="2">
+        <v>37.256998590000002</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.4449430999999999</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7.5810463800000001</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3.3294819999999999E-3</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.2368686431</v>
+      </c>
+      <c r="J9" s="2">
+        <v>2.6318738119999998</v>
+      </c>
+      <c r="K9" s="2">
+        <v>98.671319999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3.2040829</v>
+      </c>
+      <c r="C10" s="2">
+        <v>32.233413949999999</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.17710670000000001</v>
+      </c>
+      <c r="E10" s="2">
+        <v>11.98645436</v>
+      </c>
+      <c r="F10" s="2">
+        <v>3.8633741700000002</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.1187851379</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1.319834865</v>
+      </c>
+      <c r="K10" s="2">
+        <v>99.991150000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="2">
+        <v>24.697696499999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4.5971023999999998</v>
+      </c>
+      <c r="D11" s="2">
+        <v>11.216142899999999</v>
+      </c>
+      <c r="E11" s="2">
+        <v>8.9341009999999998E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3.303337923</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="2">
+        <v>7.9642269999999999E-4</v>
+      </c>
+      <c r="J11" s="2">
+        <v>8.8491409999999996E-3</v>
+      </c>
+      <c r="K11" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2.2899169999999998E-3</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-0.121881514</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0.1174578</v>
+      </c>
+      <c r="F15" s="5">
+        <v>-0.20621714999999999</v>
+      </c>
+      <c r="G15" s="5">
+        <v>5.631328E-2</v>
+      </c>
+      <c r="H15" s="5">
+        <v>-0.13095334</v>
+      </c>
+      <c r="I15" s="5">
+        <v>-0.13048601000000001</v>
+      </c>
+      <c r="J15" s="5">
+        <v>-0.56644746999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2.2899169999999998E-3</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4.4099302999999999E-2</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0.20655190000000001</v>
+      </c>
+      <c r="F16" s="5">
+        <v>-0.16659321999999999</v>
+      </c>
+      <c r="G16" s="5">
+        <v>-6.2880290000000005E-2</v>
+      </c>
+      <c r="H16" s="5">
+        <v>-3.155554E-2</v>
+      </c>
+      <c r="I16" s="5">
+        <v>-0.22007877300000001</v>
+      </c>
+      <c r="J16" s="5">
+        <v>9.5595459999999993E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="5">
+        <v>-0.121881514</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4.4099302999999999E-2</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>-0.2388594</v>
+      </c>
+      <c r="F17" s="5">
+        <v>-0.50828541999999999</v>
+      </c>
+      <c r="G17" s="5">
+        <v>9.6071069999999995E-2</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.22108374</v>
+      </c>
+      <c r="I17" s="5">
+        <v>5.8207019999999996E-3</v>
+      </c>
+      <c r="J17" s="5">
+        <v>-0.35807778000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.117457776</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.206551922</v>
+      </c>
+      <c r="D18" s="5">
+        <v>-0.238859448</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="5">
+        <v>-0.60885473000000001</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.10753428</v>
+      </c>
+      <c r="H18" s="5">
+        <v>-0.30858191000000001</v>
+      </c>
+      <c r="I18" s="5">
+        <v>-0.311970256</v>
+      </c>
+      <c r="J18" s="5">
+        <v>-0.15959244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="5">
+        <v>-0.20621715099999999</v>
+      </c>
+      <c r="C19" s="5">
+        <v>-0.16659321699999999</v>
+      </c>
+      <c r="D19" s="5">
+        <v>-0.50828542099999996</v>
+      </c>
+      <c r="E19" s="5">
+        <v>-0.60885469999999997</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>-0.28621538000000002</v>
+      </c>
+      <c r="H19" s="5">
+        <v>-0.18233057</v>
+      </c>
+      <c r="I19" s="5">
+        <v>-5.5162941E-2</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0.57506654999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5.6313283999999998E-2</v>
+      </c>
+      <c r="C20" s="5">
+        <v>-6.2880288000000006E-2</v>
+      </c>
+      <c r="D20" s="5">
+        <v>9.6071073000000007E-2</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.1075343</v>
+      </c>
+      <c r="F20" s="5">
+        <v>-0.28621538000000002</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5">
+        <v>-9.2006389999999993E-2</v>
+      </c>
+      <c r="I20" s="5">
+        <v>-6.6827253000000003E-2</v>
+      </c>
+      <c r="J20" s="5">
+        <v>-0.23447956</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="5">
+        <v>-0.130953343</v>
+      </c>
+      <c r="C21" s="5">
+        <v>-3.1555543999999998E-2</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.221083742</v>
+      </c>
+      <c r="E21" s="5">
+        <v>-0.30858190000000002</v>
+      </c>
+      <c r="F21" s="5">
+        <v>-0.18233057</v>
+      </c>
+      <c r="G21" s="5">
+        <v>-9.2006389999999993E-2</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0.83872117000000002</v>
+      </c>
+      <c r="J21" s="5">
+        <v>-9.4293790000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="5">
+        <v>-0.13048601000000001</v>
+      </c>
+      <c r="C22" s="5">
+        <v>-0.22007877300000001</v>
+      </c>
+      <c r="D22" s="5">
+        <v>5.8207019999999996E-3</v>
+      </c>
+      <c r="E22" s="5">
+        <v>-0.31197029999999998</v>
+      </c>
+      <c r="F22" s="5">
+        <v>-5.5162940000000001E-2</v>
+      </c>
+      <c r="G22" s="5">
+        <v>-6.6827250000000005E-2</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.83872117000000002</v>
+      </c>
+      <c r="I22" s="5">
+        <v>1</v>
+      </c>
+      <c r="J22" s="5">
+        <v>-1.5924250000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="5">
+        <v>-0.56644746700000004</v>
+      </c>
+      <c r="C23" s="5">
+        <v>9.5595458999999994E-2</v>
+      </c>
+      <c r="D23" s="5">
+        <v>-0.35807778299999998</v>
+      </c>
+      <c r="E23" s="5">
+        <v>-0.1595924</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.57506654999999995</v>
+      </c>
+      <c r="G23" s="5">
+        <v>-0.23447956</v>
+      </c>
+      <c r="H23" s="5">
+        <v>-9.4293790000000002E-2</v>
+      </c>
+      <c r="I23" s="5">
+        <v>-1.5924252999999999E-2</v>
+      </c>
+      <c r="J23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:F11">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:J23">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
glmm and mcmc models preliminary scripts
</commit_message>
<xml_diff>
--- a/results/Oil preliminary/PCA/exploratory PCA results.xlsx
+++ b/results/Oil preliminary/PCA/exploratory PCA results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Oilcontent_Longevity/results/Oil preliminary/PCA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="8_{52EB940A-A855-4E62-9993-921735BE7F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F53B8E6A-26DA-48CD-A7AC-BCA68EBB1EA2}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="8_{52EB940A-A855-4E62-9993-921735BE7F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5FDF3E5-3871-48A5-8879-A2A3EC26441A}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{12EB29D1-3BF5-4131-9DFF-385521089C46}"/>
   </bookViews>
@@ -362,17 +362,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,6 +877,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
@@ -1194,10 +1196,10 @@
       <c r="A1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1222,8 +1224,8 @@
       <c r="I2" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -3396,53 +3398,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="8" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="J1:J2"/>
@@ -9204,7 +9206,7 @@
   <dimension ref="A1:W25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="H14" sqref="H14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9213,11 +9215,11 @@
       <c r="A1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -9233,19 +9235,19 @@
       <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="1"/>
       <c r="I2" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="2">
@@ -9263,7 +9265,7 @@
       <c r="F3" s="2">
         <v>12.780138355</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I3" s="2">
@@ -9277,7 +9279,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="2">
@@ -9295,7 +9297,7 @@
       <c r="F4" s="2">
         <v>16.708949452999999</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="I4" s="2">
@@ -9309,7 +9311,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="2">
@@ -9327,7 +9329,7 @@
       <c r="F5" s="2">
         <v>9.2068527489999994</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="1" t="s">
         <v>57</v>
       </c>
       <c r="I5" s="2">
@@ -9341,7 +9343,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="2">
@@ -9359,7 +9361,7 @@
       <c r="F6" s="2">
         <v>10.968075292</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="1" t="s">
         <v>58</v>
       </c>
       <c r="I6" s="2">
@@ -9373,7 +9375,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="2">
@@ -9391,7 +9393,7 @@
       <c r="F7" s="2">
         <v>1.357374557</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="1" t="s">
         <v>59</v>
       </c>
       <c r="I7" s="2">
@@ -9405,7 +9407,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="2">
@@ -9423,7 +9425,7 @@
       <c r="F8" s="2">
         <v>41.808568018999999</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="1" t="s">
         <v>60</v>
       </c>
       <c r="I8" s="2">
@@ -9437,7 +9439,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B9" s="2">
@@ -9455,7 +9457,7 @@
       <c r="F9" s="2">
         <v>3.3294819999999999E-3</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="1" t="s">
         <v>61</v>
       </c>
       <c r="I9" s="2">
@@ -9469,7 +9471,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="2">
@@ -9487,7 +9489,7 @@
       <c r="F10" s="2">
         <v>3.8633741700000002</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="1" t="s">
         <v>62</v>
       </c>
       <c r="I10" s="2">
@@ -9501,7 +9503,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="2">
@@ -9519,7 +9521,7 @@
       <c r="F11" s="2">
         <v>3.303337923</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="1" t="s">
         <v>63</v>
       </c>
       <c r="I11" s="2">
@@ -9538,11 +9540,11 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="1"/>
+      <c r="B14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D14" t="s">
@@ -9557,10 +9559,10 @@
       <c r="G14" t="s">
         <v>46</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="4" t="s">
         <v>50</v>
       </c>
       <c r="J14" t="s">
@@ -9568,7 +9570,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="5">
@@ -9600,7 +9602,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="5">
@@ -9632,7 +9634,7 @@
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="5">
@@ -9664,7 +9666,7 @@
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B18" s="5">
@@ -9696,7 +9698,7 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="5">
@@ -9728,7 +9730,7 @@
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="5">
@@ -9760,7 +9762,7 @@
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="5">
@@ -9792,7 +9794,7 @@
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="5">
@@ -9824,7 +9826,7 @@
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="5">
@@ -9856,29 +9858,29 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:F11">

</xml_diff>